<commit_message>
Add residency matching data for 2024 and 2025
</commit_message>
<xml_diff>
--- a/24.xlsx
+++ b/24.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDD4705-C90F-4A9E-BF6C-1C791B011351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77169DB-9AE3-408C-91AD-ECC83E977706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9C3EA768-99BA-4CBD-BA53-289AFBACAE9C}"/>
   </bookViews>
@@ -748,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65F6E80C-5E0A-42EA-8A37-621F3AF088BC}">
   <dimension ref="A1:C545"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J551" sqref="J551"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1503,7 +1503,7 @@
         <v>0</v>
       </c>
       <c r="C68" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -1613,7 +1613,7 @@
         <v>0</v>
       </c>
       <c r="C78" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>